<commit_message>
Enhance browser security and configuration in TikTok Search Tool. Updated Chrome options for improved security, including disabling automation features and enabling secure browsing settings. Modified browser configuration parameters for better performance and security. Added tests for Chrome security configuration and login behavior to ensure robust functionality.
</commit_message>
<xml_diff>
--- a/tiktok_search_dance.xlsx
+++ b/tiktok_search_dance.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -422,9 +422,9 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="50" customWidth="1" min="1" max="1"/>
-    <col width="16" customWidth="1" min="2" max="2"/>
+    <col width="23" customWidth="1" min="2" max="2"/>
     <col width="21" customWidth="1" min="3" max="3"/>
-    <col width="26" customWidth="1" min="4" max="4"/>
+    <col width="33" customWidth="1" min="4" max="4"/>
     <col width="14" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
@@ -458,22 +458,22 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>https://www.tiktok.com/@wnyashclips2.0/video/7542195253478984982</t>
+          <t>https://www.tiktok.com/@notellieyong/video/7544270475828940037</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>wnyashclips2.0</t>
+          <t>notellieyong</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>7542195253478984982</t>
+          <t>7544270475828940037</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Video by @wnyashclips2.0</t>
+          <t>Video by @notellieyong</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -485,22 +485,22 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>https://www.tiktok.com/@kashishh.xx/video/7544014063240514822</t>
+          <t>https://www.tiktok.com/@vlea20/video/7537390559388814614</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>kashishh.xx</t>
+          <t>vlea20</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>7544014063240514822</t>
+          <t>7537390559388814614</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Video by @kashishh.xx</t>
+          <t>Video by @vlea20</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -512,22 +512,22 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>https://www.tiktok.com/@notellieyong/video/7544270475828940037</t>
+          <t>https://www.tiktok.com/@el1epretty/video/7542556415735483655</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>notellieyong</t>
+          <t>el1epretty</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>7544270475828940037</t>
+          <t>7542556415735483655</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Video by @notellieyong</t>
+          <t>Video by @el1epretty</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -566,22 +566,22 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>https://www.tiktok.com/@evaforevahh/video/7544114446122224904</t>
+          <t>https://www.tiktok.com/@maligoshik/video/7541181053327740168</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>evaforevahh</t>
+          <t>maligoshik</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>7544114446122224904</t>
+          <t>7541181053327740168</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Video by @evaforevahh</t>
+          <t>Video by @maligoshik</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -593,25 +593,403 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>https://www.tiktok.com/@mayaa.zrr/video/7544392636782660886</t>
+          <t>https://www.tiktok.com/@shaniaandmads/video/7542457398993145095</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>mayaa.zrr</t>
+          <t>shaniaandmads</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>7544392636782660886</t>
+          <t>7542457398993145095</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Video by @mayaa.zrr</t>
+          <t>Video by @shaniaandmads</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
+        <is>
+          <t>dance</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>https://www.tiktok.com/@n_clarissa/video/7544383024348122390</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>n_clarissa</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>7544383024348122390</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Video by @n_clarissa</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>dance</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>https://www.tiktok.com/@evaforevahh/video/7544114446122224904</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>evaforevahh</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>7544114446122224904</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Video by @evaforevahh</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>dance</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>https://www.tiktok.com/@celynbrook.dance/video/7542963317246135574</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>celynbrook.dance</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>7542963317246135574</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Video by @celynbrook.dance</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>dance</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>https://www.tiktok.com/@wnyashclips2.0/video/7542195253478984982</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>wnyashclips2.0</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>7542195253478984982</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Video by @wnyashclips2.0</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>dance</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>https://www.tiktok.com/@zhurtik/video/7512543844957687045</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>zhurtik</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>7512543844957687045</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Video by @zhurtik</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>dance</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>https://www.tiktok.com/@ari.5369/video/7539280922726714646</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>ari.5369</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>7539280922726714646</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Video by @ari.5369</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>dance</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>https://www.tiktok.com/@el1epretty/video/7540703940527017223</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>el1epretty</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>7540703940527017223</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Video by @el1epretty</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>dance</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>https://www.tiktok.com/@lxttikaem1ly/video/7541740945637936407</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>lxttikaem1ly</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>7541740945637936407</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Video by @lxttikaem1ly</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>dance</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>https://www.tiktok.com/@baddiesofticktok/video/7540557654746270998</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>baddiesofticktok</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>7540557654746270998</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Video by @baddiesofticktok</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>dance</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>https://www.tiktok.com/@cocolu.xx/video/7523461069449301278</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>cocolu.xx</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>7523461069449301278</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Video by @cocolu.xx</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>dance</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>https://www.tiktok.com/@pla_neii/video/7543961522771430663</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>pla_neii</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>7543961522771430663</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Video by @pla_neii</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>dance</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>https://www.tiktok.com/@sadieemckennaa/video/7404604972358241542</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>sadieemckennaa</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>7404604972358241542</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Video by @sadieemckennaa</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>dance</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>https://www.tiktok.com/@dancingbabies_t.and.j/video/7514894090413231406</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>dancingbabies_t.and.j</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>7514894090413231406</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Video by @dancingbabies_t.and.j</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>dance</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>https://www.tiktok.com/@sara.guglielmetto/video/7540945564918107414</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>sara.guglielmetto</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>7540945564918107414</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Video by @sara.guglielmetto</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
         <is>
           <t>dance</t>
         </is>

</xml_diff>